<commit_message>
new datamaker and small new data
</commit_message>
<xml_diff>
--- a/experiment/ParameterRecord.xlsx
+++ b/experiment/ParameterRecord.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Change\Research\StochasticPricingModelSayanMukherjee\experiment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zd26\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BC887B-1255-44F9-8467-55CF5EF76D9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B88AF14-4D69-4BF1-A287-A35C2FAD4A3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{F73232D0-7E87-476B-ADE1-6A31317C3E7A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
   <si>
     <t>date range</t>
   </si>
@@ -119,12 +119,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D57E9EB-BEEF-4020-81F2-1012D35CE26B}">
-  <dimension ref="B1:M21"/>
+  <dimension ref="B1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -500,194 +504,47 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>50</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>0.4</v>
-      </c>
-      <c r="G2">
-        <v>0.98</v>
-      </c>
-      <c r="H2">
+    <row r="2" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.34289999999999998</v>
+      </c>
+      <c r="M2" s="1">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E3" s="4">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0.34189999999999998</v>
+      </c>
+      <c r="M3" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E4" s="4">
         <v>5</v>
       </c>
-      <c r="I2">
-        <v>-7</v>
-      </c>
-      <c r="J2">
-        <v>100</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <v>0.3427</v>
-      </c>
-      <c r="M2">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>0.4</v>
-      </c>
-      <c r="G3">
-        <v>0.98</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>-7</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-      <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3">
-        <v>0.34250000000000003</v>
-      </c>
-      <c r="M3">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>50</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>0.4</v>
-      </c>
-      <c r="G4">
-        <v>0.98</v>
-      </c>
-      <c r="H4">
-        <v>5</v>
-      </c>
-      <c r="I4">
-        <v>-7</v>
-      </c>
-      <c r="J4">
-        <v>100</v>
-      </c>
-      <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4">
-        <v>0.34250000000000003</v>
-      </c>
-      <c r="M4">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>0.4</v>
-      </c>
-      <c r="G5">
-        <v>0.98</v>
-      </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-      <c r="I5">
-        <v>-7</v>
-      </c>
-      <c r="J5">
-        <v>100</v>
-      </c>
-      <c r="K5">
-        <v>4</v>
-      </c>
-      <c r="L5">
-        <v>0.34250000000000003</v>
-      </c>
-      <c r="M5">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>14</v>
-      </c>
-      <c r="F6">
-        <v>0.4</v>
-      </c>
-      <c r="G6">
-        <v>0.98</v>
-      </c>
-      <c r="H6">
-        <v>5</v>
-      </c>
-      <c r="I6">
-        <v>-7</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-      <c r="K6">
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <v>0.34250000000000003</v>
-      </c>
-      <c r="M6">
-        <v>58</v>
+      <c r="L4" s="1">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M4" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.55000000000000004">
@@ -701,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="E7">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>0.4</v>
@@ -722,10 +579,10 @@
         <v>4</v>
       </c>
       <c r="L7">
-        <v>0.34239999999999998</v>
+        <v>0.3427</v>
       </c>
       <c r="M7">
-        <v>29</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.55000000000000004">
@@ -739,7 +596,7 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F8">
         <v>0.4</v>
@@ -763,7 +620,7 @@
         <v>0.34250000000000003</v>
       </c>
       <c r="M8">
-        <v>94</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.55000000000000004">
@@ -777,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="E9">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>0.4</v>
@@ -798,10 +655,10 @@
         <v>4</v>
       </c>
       <c r="L9">
-        <v>0.34239999999999998</v>
+        <v>0.34250000000000003</v>
       </c>
       <c r="M9">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.55000000000000004">
@@ -815,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="E10">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <v>0.4</v>
@@ -836,10 +693,10 @@
         <v>4</v>
       </c>
       <c r="L10">
-        <v>0.34239999999999998</v>
+        <v>0.34250000000000003</v>
       </c>
       <c r="M10">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.55000000000000004">
@@ -853,7 +710,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F11">
         <v>0.4</v>
@@ -874,105 +731,656 @@
         <v>4</v>
       </c>
       <c r="L11">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>0.4</v>
+      </c>
+      <c r="G12">
+        <v>0.98</v>
+      </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>-7</v>
+      </c>
+      <c r="J12">
+        <v>100</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
         <v>0.34239999999999998</v>
       </c>
-      <c r="M11">
+      <c r="M12">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>0.4</v>
+      </c>
+      <c r="G13">
+        <v>0.98</v>
+      </c>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>-7</v>
+      </c>
+      <c r="J13">
+        <v>100</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M13">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>19</v>
+      </c>
+      <c r="F14">
+        <v>0.4</v>
+      </c>
+      <c r="G14">
+        <v>0.98</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <v>-7</v>
+      </c>
+      <c r="J14">
+        <v>100</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>0.34239999999999998</v>
+      </c>
+      <c r="M14">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2">
-        <v>50</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>50</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>21</v>
+      </c>
+      <c r="F15">
+        <v>0.4</v>
+      </c>
+      <c r="G15">
+        <v>0.98</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>-7</v>
+      </c>
+      <c r="J15">
+        <v>100</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>0.34239999999999998</v>
+      </c>
+      <c r="M15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <v>0.4</v>
+      </c>
+      <c r="G16">
+        <v>0.98</v>
+      </c>
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>-7</v>
+      </c>
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16">
+        <v>0.34239999999999998</v>
+      </c>
+      <c r="M16">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2">
+        <v>50</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+      <c r="E17" s="2">
         <v>16</v>
       </c>
-      <c r="F12" s="2">
-        <v>0.4</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.98</v>
-      </c>
-      <c r="H12" s="2">
+      <c r="F17" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="H17" s="2">
         <v>5</v>
       </c>
-      <c r="I12" s="2">
-        <v>-7</v>
-      </c>
-      <c r="J12" s="2">
-        <v>100</v>
-      </c>
-      <c r="K12" s="2">
-        <v>4</v>
-      </c>
-      <c r="L12" s="2">
+      <c r="I17" s="2">
+        <v>-7</v>
+      </c>
+      <c r="J17" s="2">
+        <v>100</v>
+      </c>
+      <c r="K17" s="2">
+        <v>4</v>
+      </c>
+      <c r="L17" s="2">
         <v>0.34210000000000002</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M17" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="H13">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3">
+        <v>50</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>16</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H18">
         <v>0.5</v>
       </c>
-      <c r="L13">
-        <v>0.34250000000000003</v>
-      </c>
-      <c r="M13">
+      <c r="I18" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J18" s="3">
+        <v>100</v>
+      </c>
+      <c r="K18" s="3">
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M18">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="H14">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="3">
+        <v>50</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>16</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H19">
         <v>1</v>
       </c>
-      <c r="L14">
-        <v>0.34250000000000003</v>
-      </c>
-      <c r="M14">
+      <c r="I19" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J19" s="3">
+        <v>100</v>
+      </c>
+      <c r="K19" s="3">
+        <v>4</v>
+      </c>
+      <c r="L19">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M19">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="H15">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="3">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>16</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H20">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="H16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="H17">
+      <c r="I20" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J20" s="3">
+        <v>100</v>
+      </c>
+      <c r="K20" s="3">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M20">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="3">
+        <v>50</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>16</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J21" s="3">
+        <v>100</v>
+      </c>
+      <c r="K21" s="3">
+        <v>4</v>
+      </c>
+      <c r="L21">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M21">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="3">
+        <v>50</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>16</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H22">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="H18">
+      <c r="I22" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J22" s="3">
+        <v>100</v>
+      </c>
+      <c r="K22" s="3">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="3">
+        <v>50</v>
+      </c>
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>16</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H23">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="H19">
+      <c r="I23" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J23" s="3">
+        <v>100</v>
+      </c>
+      <c r="K23" s="3">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M23">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="H20">
+      <c r="F24" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H24">
+        <v>16</v>
+      </c>
+      <c r="I24" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J24" s="3">
+        <v>100</v>
+      </c>
+      <c r="K24" s="3">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M24">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="3">
+        <v>50</v>
+      </c>
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>16</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H25">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="H21">
-        <v>24</v>
+      <c r="I25" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J25" s="3">
+        <v>100</v>
+      </c>
+      <c r="K25" s="3">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3">
+        <v>50</v>
+      </c>
+      <c r="D26" s="3">
+        <v>2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>16</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H26">
+        <v>40</v>
+      </c>
+      <c r="I26" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J26" s="3">
+        <v>100</v>
+      </c>
+      <c r="K26" s="3">
+        <v>4</v>
+      </c>
+      <c r="L26">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M26">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="3">
+        <v>50</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>16</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H27">
+        <v>70</v>
+      </c>
+      <c r="I27" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J27" s="3">
+        <v>100</v>
+      </c>
+      <c r="K27" s="3">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M27">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3">
+        <v>50</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>16</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
+      <c r="I28" s="3">
+        <v>-7</v>
+      </c>
+      <c r="J28" s="3">
+        <v>100</v>
+      </c>
+      <c r="K28" s="3">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>0.34250000000000003</v>
+      </c>
+      <c r="M28">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>